<commit_message>
Made minor change in user test case 1 :wq
</commit_message>
<xml_diff>
--- a/ProjectCP_3/TestCase1_datadisplay.xlsx
+++ b/ProjectCP_3/TestCase1_datadisplay.xlsx
@@ -427,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -606,6 +606,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -941,7 +947,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:F27"/>
+      <selection activeCell="A28" sqref="A28:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1264,10 +1270,10 @@
       <c r="H27" s="21"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="11"/>
+      <c r="B28" s="64"/>
       <c r="C28" s="26" t="s">
         <v>24</v>
       </c>
@@ -1278,8 +1284,8 @@
       <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="10"/>
-      <c r="B29" s="11"/>
+      <c r="A29" s="63"/>
+      <c r="B29" s="64"/>
       <c r="C29" s="26"/>
       <c r="D29" s="27"/>
       <c r="E29" s="14"/>

</xml_diff>

<commit_message>
Added project 3 finishing touches.TM
</commit_message>
<xml_diff>
--- a/ProjectCP_3/TestCase1_datadisplay.xlsx
+++ b/ProjectCP_3/TestCase1_datadisplay.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24640" windowHeight="15560" tabRatio="500"/>
   </bookViews>
@@ -427,60 +427,56 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -502,102 +498,90 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -607,11 +591,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -946,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B29"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -962,479 +946,481 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="62"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
-      <c r="E2" s="62"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="62"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
+      <c r="A3" s="54"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
+      <c r="A4" s="54"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="62"/>
-      <c r="B5" s="62"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="60"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60" t="s">
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="60"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
+      <c r="G9" s="53"/>
+      <c r="H9" s="53"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="60" t="s">
+      <c r="B10" s="53"/>
+      <c r="C10" s="53"/>
+      <c r="D10" s="53"/>
+      <c r="E10" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="61"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
-      <c r="H11" s="60"/>
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="60" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="60"/>
-      <c r="G12" s="60"/>
-      <c r="H12" s="60"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="61"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="46"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="47"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="50"/>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="41"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="55"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="44"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="55"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="44"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="49"/>
+      <c r="C20" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="29" t="s">
+      <c r="D20" s="49"/>
+      <c r="E20" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="30"/>
-      <c r="G20" s="58" t="s">
+      <c r="F20" s="46"/>
+      <c r="G20" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H20" s="56" t="s">
+      <c r="H20" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="3"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="59"/>
-      <c r="H21" s="57"/>
+      <c r="A21" s="56"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="46"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1">
-      <c r="A22" s="33" t="s">
+      <c r="A22" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="33" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="34"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="40"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="35"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="26" t="s">
+      <c r="B24" s="23"/>
+      <c r="C24" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="22"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="42"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="A25" s="22"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="36"/>
-      <c r="C26" s="37" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="35"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="63" t="s">
+      <c r="A28" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="26" t="s">
+      <c r="B28" s="23"/>
+      <c r="C28" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="63"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="A29" s="22"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="8"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="10"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="10"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="18"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="8"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="10"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="22"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="10"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="22"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="8"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="18"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
+      <c r="A39" s="16"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="11"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
+      <c r="A40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="12"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="68">
+    <mergeCell ref="C20:D21"/>
+    <mergeCell ref="A20:B21"/>
     <mergeCell ref="E6:H7"/>
     <mergeCell ref="E8:H9"/>
     <mergeCell ref="E10:H11"/>

</xml_diff>